<commit_message>
fix leading 0 zip codes
</commit_message>
<xml_diff>
--- a/datasource/Field Marketing Philly Zips.xlsx
+++ b/datasource/Field Marketing Philly Zips.xlsx
@@ -5,19 +5,16 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/percyli/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/percyli/Desktop/swan work/ABikeride/zipcode/2022 heatmap/datasource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81BF18F-645F-1A4C-998D-BA3BE4F9CB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229F916B-24A3-3C43-8F4D-602BE5C362D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="500" windowWidth="25620" windowHeight="17500" tabRatio="774" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27540" yWindow="3220" windowWidth="25620" windowHeight="17500" tabRatio="774" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zip Codes Field Marketing " sheetId="11" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Zip Codes Field Marketing '!$A$1:$A$1634</definedName>
-  </definedNames>
   <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -598,7 +595,7 @@
   <dimension ref="A1:A1634"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D911" sqref="D911"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,7 +603,7 @@
     <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8777,11 +8774,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1634" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A1781">
-      <sortCondition descending="1" ref="A1:A1781"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>